<commit_message>
remove special char in Unit values
</commit_message>
<xml_diff>
--- a/Coraltraits/coraltraits_mapping.xlsx
+++ b/Coraltraits/coraltraits_mapping.xlsx
@@ -1222,7 +1222,15 @@
     <t>¬µm cm^-2 h^-1</t>
   </si>
   <si>
-    <t>http://eol.org/schema/terms/Âµmol_cm-2_hr-1</t>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="13"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>http://eol.org/schema/terms/µmol_cm-2_hr-1</t>
+    </r>
   </si>
   <si>
     <t>¬µmol O2 cm^-2 h^-1</t>
@@ -1231,7 +1239,15 @@
     <t>¬µmol quanta m^-2 s^-1</t>
   </si>
   <si>
-    <t>http://eol.org/schema/terms/Âµmol_m-2_s-1</t>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="13"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>http://eol.org/schema/terms/µmol_m-2_s-1</t>
+    </r>
   </si>
   <si>
     <t>0/00</t>
@@ -1436,7 +1452,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -1456,6 +1472,12 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="12"/>
+      <color indexed="13"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1641,7 +1663,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -1651,7 +1673,7 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1670,9 +1692,6 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1696,25 +1715,16 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1744,6 +1754,7 @@
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffffff00"/>
       <rgbColor rgb="ffbfbfbf"/>
+      <rgbColor rgb="ff0000ff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1942,17 +1953,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1980,10 +1991,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -2231,12 +2242,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -2523,7 +2534,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -2551,10 +2562,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -3034,7 +3045,7 @@
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
-      <c r="Q2" s="10"/>
+      <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
       <c r="S2" s="3"/>
       <c r="T2" s="3"/>
@@ -3047,7 +3058,7 @@
       <c r="AA2" s="3"/>
       <c r="AB2" s="3"/>
       <c r="AC2" s="3"/>
-      <c r="AD2" s="10"/>
+      <c r="AD2" s="3"/>
     </row>
     <row r="3" ht="17" customHeight="1">
       <c r="A3" t="s" s="2">
@@ -3056,7 +3067,7 @@
       <c r="B3" t="s" s="2">
         <v>17</v>
       </c>
-      <c r="C3" s="10"/>
+      <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -3064,15 +3075,15 @@
       <c r="H3" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="I3" s="10"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="10"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
-      <c r="Q3" s="10"/>
+      <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
@@ -3085,7 +3096,7 @@
       <c r="AA3" s="3"/>
       <c r="AB3" s="3"/>
       <c r="AC3" s="3"/>
-      <c r="AD3" s="10"/>
+      <c r="AD3" s="3"/>
     </row>
     <row r="4" ht="17" customHeight="1">
       <c r="A4" t="s" s="2">
@@ -3094,7 +3105,7 @@
       <c r="B4" t="s" s="2">
         <v>25</v>
       </c>
-      <c r="C4" s="10"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -3108,7 +3119,7 @@
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
-      <c r="Q4" s="10"/>
+      <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
@@ -3121,7 +3132,7 @@
       <c r="AA4" s="3"/>
       <c r="AB4" s="3"/>
       <c r="AC4" s="3"/>
-      <c r="AD4" s="10"/>
+      <c r="AD4" s="3"/>
     </row>
     <row r="5" ht="17" customHeight="1">
       <c r="A5" t="s" s="2">
@@ -3130,7 +3141,7 @@
       <c r="B5" t="s" s="2">
         <v>13</v>
       </c>
-      <c r="C5" s="10"/>
+      <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -3144,7 +3155,7 @@
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
-      <c r="Q5" s="10"/>
+      <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
       <c r="T5" s="3"/>
@@ -3157,7 +3168,7 @@
       <c r="AA5" s="3"/>
       <c r="AB5" s="3"/>
       <c r="AC5" s="3"/>
-      <c r="AD5" s="10"/>
+      <c r="AD5" s="3"/>
     </row>
     <row r="6" ht="17" customHeight="1">
       <c r="A6" t="s" s="2">
@@ -3166,7 +3177,7 @@
       <c r="B6" t="s" s="2">
         <v>28</v>
       </c>
-      <c r="C6" s="10"/>
+      <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -3180,7 +3191,7 @@
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
-      <c r="Q6" s="10"/>
+      <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
@@ -3193,7 +3204,7 @@
       <c r="AA6" s="3"/>
       <c r="AB6" s="3"/>
       <c r="AC6" s="3"/>
-      <c r="AD6" s="10"/>
+      <c r="AD6" s="3"/>
     </row>
     <row r="7" ht="17" customHeight="1">
       <c r="A7" t="s" s="2">
@@ -3202,7 +3213,7 @@
       <c r="B7" t="s" s="2">
         <v>30</v>
       </c>
-      <c r="C7" s="10"/>
+      <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -3216,7 +3227,7 @@
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
-      <c r="Q7" s="10"/>
+      <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
@@ -3229,7 +3240,7 @@
       <c r="AA7" s="3"/>
       <c r="AB7" s="3"/>
       <c r="AC7" s="3"/>
-      <c r="AD7" s="10"/>
+      <c r="AD7" s="3"/>
     </row>
     <row r="8" ht="17" customHeight="1">
       <c r="A8" t="s" s="2">
@@ -3238,7 +3249,7 @@
       <c r="B8" t="s" s="2">
         <v>32</v>
       </c>
-      <c r="C8" s="10"/>
+      <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -3252,7 +3263,7 @@
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
-      <c r="Q8" s="10"/>
+      <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
@@ -3265,13 +3276,13 @@
       <c r="AA8" s="3"/>
       <c r="AB8" s="3"/>
       <c r="AC8" s="3"/>
-      <c r="AD8" s="10"/>
+      <c r="AD8" s="3"/>
     </row>
     <row r="9" ht="17" customHeight="1">
       <c r="A9" t="s" s="2">
         <v>33</v>
       </c>
-      <c r="B9" t="s" s="12">
+      <c r="B9" t="s" s="11">
         <v>34</v>
       </c>
       <c r="C9" s="6"/>
@@ -3288,7 +3299,7 @@
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
-      <c r="Q9" s="10"/>
+      <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
@@ -3301,7 +3312,7 @@
       <c r="AA9" s="3"/>
       <c r="AB9" s="3"/>
       <c r="AC9" s="3"/>
-      <c r="AD9" s="10"/>
+      <c r="AD9" s="3"/>
     </row>
     <row r="10" ht="17" customHeight="1">
       <c r="A10" t="s" s="2">
@@ -3310,7 +3321,7 @@
       <c r="B10" t="s" s="2">
         <v>36</v>
       </c>
-      <c r="C10" s="10"/>
+      <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" t="s" s="2">
@@ -3319,16 +3330,16 @@
       <c r="G10" t="s" s="2">
         <v>38</v>
       </c>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
-      <c r="Q10" s="10"/>
+      <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
@@ -3341,7 +3352,7 @@
       <c r="AA10" s="3"/>
       <c r="AB10" s="3"/>
       <c r="AC10" s="3"/>
-      <c r="AD10" s="10"/>
+      <c r="AD10" s="3"/>
     </row>
     <row r="11" ht="17" customHeight="1">
       <c r="A11" t="s" s="2">
@@ -3350,7 +3361,7 @@
       <c r="B11" t="s" s="2">
         <v>28</v>
       </c>
-      <c r="C11" s="10"/>
+      <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -3364,7 +3375,7 @@
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
-      <c r="Q11" s="10"/>
+      <c r="Q11" s="3"/>
       <c r="R11" s="3"/>
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
@@ -3377,7 +3388,7 @@
       <c r="AA11" s="3"/>
       <c r="AB11" s="3"/>
       <c r="AC11" s="3"/>
-      <c r="AD11" s="10"/>
+      <c r="AD11" s="3"/>
     </row>
     <row r="12" ht="17" customHeight="1">
       <c r="A12" t="s" s="2">
@@ -3386,7 +3397,7 @@
       <c r="B12" t="s" s="2">
         <v>41</v>
       </c>
-      <c r="C12" s="10"/>
+      <c r="C12" s="3"/>
       <c r="D12" t="s" s="2">
         <v>42</v>
       </c>
@@ -3394,17 +3405,17 @@
       <c r="F12" t="s" s="2">
         <v>37</v>
       </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
-      <c r="Q12" s="10"/>
+      <c r="Q12" s="3"/>
       <c r="R12" s="3"/>
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
@@ -3426,7 +3437,7 @@
       <c r="B13" t="s" s="2">
         <v>13</v>
       </c>
-      <c r="C13" s="10"/>
+      <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -3440,7 +3451,7 @@
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
-      <c r="Q13" s="10"/>
+      <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
@@ -3462,7 +3473,7 @@
       <c r="B14" t="s" s="2">
         <v>36</v>
       </c>
-      <c r="C14" s="10"/>
+      <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" t="s" s="2">
@@ -3480,7 +3491,7 @@
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
-      <c r="Q14" s="10"/>
+      <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
@@ -3502,7 +3513,7 @@
       <c r="B15" t="s" s="2">
         <v>47</v>
       </c>
-      <c r="C15" s="10"/>
+      <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" t="s" s="2">
@@ -3518,7 +3529,7 @@
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
-      <c r="Q15" s="10"/>
+      <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
@@ -3540,7 +3551,7 @@
       <c r="B16" t="s" s="2">
         <v>47</v>
       </c>
-      <c r="C16" s="10"/>
+      <c r="C16" s="3"/>
       <c r="D16" t="s" s="2">
         <v>42</v>
       </c>
@@ -3558,7 +3569,7 @@
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
-      <c r="Q16" s="10"/>
+      <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
@@ -3580,7 +3591,7 @@
       <c r="B17" t="s" s="2">
         <v>47</v>
       </c>
-      <c r="C17" s="10"/>
+      <c r="C17" s="3"/>
       <c r="D17" t="s" s="2">
         <v>51</v>
       </c>
@@ -3598,7 +3609,7 @@
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
-      <c r="Q17" s="10"/>
+      <c r="Q17" s="3"/>
       <c r="R17" s="3"/>
       <c r="S17" s="3"/>
       <c r="T17" s="3"/>
@@ -3620,7 +3631,7 @@
       <c r="B18" t="s" s="2">
         <v>53</v>
       </c>
-      <c r="C18" s="10"/>
+      <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -3634,7 +3645,7 @@
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
-      <c r="Q18" s="10"/>
+      <c r="Q18" s="3"/>
       <c r="R18" s="3"/>
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
@@ -3650,13 +3661,13 @@
       <c r="AD18" s="3"/>
     </row>
     <row r="19" ht="17" customHeight="1">
-      <c r="A19" t="s" s="13">
+      <c r="A19" t="s" s="12">
         <v>54</v>
       </c>
-      <c r="B19" t="s" s="14">
+      <c r="B19" t="s" s="13">
         <v>55</v>
       </c>
-      <c r="C19" s="15"/>
+      <c r="C19" s="14"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -3670,7 +3681,7 @@
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>
-      <c r="Q19" s="10"/>
+      <c r="Q19" s="3"/>
       <c r="R19" s="3"/>
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
@@ -3678,7 +3689,7 @@
       <c r="V19" s="3"/>
       <c r="W19" s="3"/>
       <c r="X19" s="3"/>
-      <c r="Y19" s="10"/>
+      <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
       <c r="AA19" s="3"/>
       <c r="AB19" s="3"/>
@@ -3689,10 +3700,10 @@
       <c r="A20" t="s" s="2">
         <v>56</v>
       </c>
-      <c r="B20" t="s" s="16">
+      <c r="B20" t="s" s="15">
         <v>57</v>
       </c>
-      <c r="C20" s="10"/>
+      <c r="C20" s="3"/>
       <c r="D20" t="s" s="2">
         <v>42</v>
       </c>
@@ -3716,7 +3727,7 @@
       <c r="V20" s="3"/>
       <c r="W20" s="3"/>
       <c r="X20" s="3"/>
-      <c r="Y20" s="10"/>
+      <c r="Y20" s="3"/>
       <c r="Z20" s="3"/>
       <c r="AA20" s="3"/>
       <c r="AB20" s="3"/>
@@ -3730,7 +3741,7 @@
       <c r="B21" t="s" s="2">
         <v>57</v>
       </c>
-      <c r="C21" s="10"/>
+      <c r="C21" s="3"/>
       <c r="D21" t="s" s="2">
         <v>51</v>
       </c>
@@ -3746,7 +3757,7 @@
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
       <c r="P21" s="3"/>
-      <c r="Q21" s="10"/>
+      <c r="Q21" s="3"/>
       <c r="R21" s="3"/>
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
@@ -3754,7 +3765,7 @@
       <c r="V21" s="3"/>
       <c r="W21" s="3"/>
       <c r="X21" s="3"/>
-      <c r="Y21" s="10"/>
+      <c r="Y21" s="3"/>
       <c r="Z21" s="3"/>
       <c r="AA21" s="3"/>
       <c r="AB21" s="3"/>
@@ -3768,7 +3779,7 @@
       <c r="B22" t="s" s="2">
         <v>60</v>
       </c>
-      <c r="C22" s="10"/>
+      <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -3782,7 +3793,7 @@
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
       <c r="P22" s="3"/>
-      <c r="Q22" s="10"/>
+      <c r="Q22" s="3"/>
       <c r="R22" s="3"/>
       <c r="S22" s="3"/>
       <c r="T22" s="3"/>
@@ -3790,7 +3801,7 @@
       <c r="V22" s="3"/>
       <c r="W22" s="3"/>
       <c r="X22" s="3"/>
-      <c r="Y22" s="10"/>
+      <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
       <c r="AA22" s="3"/>
       <c r="AB22" s="3"/>
@@ -3804,7 +3815,7 @@
       <c r="B23" t="s" s="2">
         <v>62</v>
       </c>
-      <c r="C23" s="10"/>
+      <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -3818,7 +3829,7 @@
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
-      <c r="Q23" s="10"/>
+      <c r="Q23" s="3"/>
       <c r="R23" s="3"/>
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
@@ -3826,7 +3837,7 @@
       <c r="V23" s="3"/>
       <c r="W23" s="3"/>
       <c r="X23" s="3"/>
-      <c r="Y23" s="10"/>
+      <c r="Y23" s="3"/>
       <c r="Z23" s="3"/>
       <c r="AA23" s="3"/>
       <c r="AB23" s="3"/>
@@ -3840,7 +3851,7 @@
       <c r="B24" t="s" s="2">
         <v>53</v>
       </c>
-      <c r="C24" s="10"/>
+      <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -3854,7 +3865,7 @@
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
-      <c r="Q24" s="10"/>
+      <c r="Q24" s="3"/>
       <c r="R24" s="3"/>
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
@@ -3892,7 +3903,7 @@
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
-      <c r="Q25" s="10"/>
+      <c r="Q25" s="3"/>
       <c r="R25" s="3"/>
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
@@ -3928,7 +3939,7 @@
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
-      <c r="Q26" s="10"/>
+      <c r="Q26" s="3"/>
       <c r="R26" s="3"/>
       <c r="S26" s="3"/>
       <c r="T26" s="3"/>
@@ -3944,13 +3955,13 @@
       <c r="AD26" s="3"/>
     </row>
     <row r="27" ht="17" customHeight="1">
-      <c r="A27" t="s" s="13">
+      <c r="A27" t="s" s="12">
         <v>68</v>
       </c>
-      <c r="B27" t="s" s="14">
+      <c r="B27" t="s" s="13">
         <v>69</v>
       </c>
-      <c r="C27" s="15"/>
+      <c r="C27" s="14"/>
       <c r="D27" t="s" s="2">
         <v>42</v>
       </c>
@@ -3966,7 +3977,7 @@
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
-      <c r="Q27" s="10"/>
+      <c r="Q27" s="3"/>
       <c r="R27" s="3"/>
       <c r="S27" s="3"/>
       <c r="T27" s="3"/>
@@ -3982,13 +3993,13 @@
       <c r="AD27" s="3"/>
     </row>
     <row r="28" ht="17" customHeight="1">
-      <c r="A28" t="s" s="13">
+      <c r="A28" t="s" s="12">
         <v>70</v>
       </c>
-      <c r="B28" t="s" s="17">
+      <c r="B28" t="s" s="16">
         <v>71</v>
       </c>
-      <c r="C28" s="18"/>
+      <c r="C28" s="14"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
@@ -4002,7 +4013,7 @@
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>
-      <c r="Q28" s="10"/>
+      <c r="Q28" s="3"/>
       <c r="R28" s="3"/>
       <c r="S28" s="3"/>
       <c r="T28" s="3"/>
@@ -4021,7 +4032,7 @@
       <c r="A29" t="s" s="2">
         <v>72</v>
       </c>
-      <c r="B29" t="s" s="16">
+      <c r="B29" t="s" s="15">
         <v>53</v>
       </c>
       <c r="C29" s="3"/>
@@ -4038,7 +4049,7 @@
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
-      <c r="Q29" s="10"/>
+      <c r="Q29" s="3"/>
       <c r="R29" s="3"/>
       <c r="S29" s="3"/>
       <c r="T29" s="3"/>
@@ -4074,7 +4085,7 @@
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
       <c r="P30" s="3"/>
-      <c r="Q30" s="10"/>
+      <c r="Q30" s="3"/>
       <c r="R30" s="3"/>
       <c r="S30" s="3"/>
       <c r="T30" s="3"/>
@@ -4096,7 +4107,7 @@
       <c r="B31" t="s" s="2">
         <v>75</v>
       </c>
-      <c r="C31" s="10"/>
+      <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
@@ -4110,7 +4121,7 @@
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>
       <c r="P31" s="3"/>
-      <c r="Q31" s="10"/>
+      <c r="Q31" s="3"/>
       <c r="R31" s="3"/>
       <c r="S31" s="3"/>
       <c r="T31" s="3"/>
@@ -4126,13 +4137,13 @@
       <c r="AD31" s="3"/>
     </row>
     <row r="32" ht="17" customHeight="1">
-      <c r="A32" t="s" s="13">
+      <c r="A32" t="s" s="12">
         <v>76</v>
       </c>
-      <c r="B32" t="s" s="14">
+      <c r="B32" t="s" s="13">
         <v>77</v>
       </c>
-      <c r="C32" s="15"/>
+      <c r="C32" s="14"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
@@ -4146,7 +4157,7 @@
       <c r="N32" s="3"/>
       <c r="O32" s="3"/>
       <c r="P32" s="3"/>
-      <c r="Q32" s="10"/>
+      <c r="Q32" s="3"/>
       <c r="R32" s="3"/>
       <c r="S32" s="3"/>
       <c r="T32" s="3"/>
@@ -4162,13 +4173,13 @@
       <c r="AD32" s="3"/>
     </row>
     <row r="33" ht="17" customHeight="1">
-      <c r="A33" t="s" s="13">
+      <c r="A33" t="s" s="12">
         <v>78</v>
       </c>
-      <c r="B33" t="s" s="17">
+      <c r="B33" t="s" s="16">
         <v>19</v>
       </c>
-      <c r="C33" s="15"/>
+      <c r="C33" s="14"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
@@ -4182,7 +4193,7 @@
       <c r="N33" s="3"/>
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
-      <c r="Q33" s="10"/>
+      <c r="Q33" s="3"/>
       <c r="R33" s="3"/>
       <c r="S33" s="3"/>
       <c r="T33" s="3"/>
@@ -4201,10 +4212,10 @@
       <c r="A34" t="s" s="2">
         <v>79</v>
       </c>
-      <c r="B34" t="s" s="16">
+      <c r="B34" t="s" s="15">
         <v>80</v>
       </c>
-      <c r="C34" s="10"/>
+      <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
@@ -4218,7 +4229,7 @@
       <c r="N34" s="3"/>
       <c r="O34" s="3"/>
       <c r="P34" s="3"/>
-      <c r="Q34" s="10"/>
+      <c r="Q34" s="3"/>
       <c r="R34" s="3"/>
       <c r="S34" s="3"/>
       <c r="T34" s="3"/>
@@ -4240,7 +4251,7 @@
       <c r="B35" t="s" s="2">
         <v>82</v>
       </c>
-      <c r="C35" s="10"/>
+      <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
@@ -4254,7 +4265,7 @@
       <c r="N35" s="3"/>
       <c r="O35" s="3"/>
       <c r="P35" s="3"/>
-      <c r="Q35" s="10"/>
+      <c r="Q35" s="3"/>
       <c r="R35" s="3"/>
       <c r="S35" s="3"/>
       <c r="T35" s="3"/>
@@ -4276,7 +4287,7 @@
       <c r="B36" t="s" s="2">
         <v>82</v>
       </c>
-      <c r="C36" s="10"/>
+      <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
@@ -4290,7 +4301,7 @@
       <c r="N36" s="3"/>
       <c r="O36" s="3"/>
       <c r="P36" s="3"/>
-      <c r="Q36" s="10"/>
+      <c r="Q36" s="3"/>
       <c r="R36" s="3"/>
       <c r="S36" s="3"/>
       <c r="T36" s="3"/>
@@ -4312,7 +4323,7 @@
       <c r="B37" t="s" s="2">
         <v>82</v>
       </c>
-      <c r="C37" s="10"/>
+      <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
@@ -4328,7 +4339,7 @@
       <c r="N37" s="3"/>
       <c r="O37" s="3"/>
       <c r="P37" s="3"/>
-      <c r="Q37" s="10"/>
+      <c r="Q37" s="3"/>
       <c r="R37" s="3"/>
       <c r="S37" s="3"/>
       <c r="T37" s="3"/>
@@ -4350,7 +4361,7 @@
       <c r="B38" t="s" s="2">
         <v>82</v>
       </c>
-      <c r="C38" s="10"/>
+      <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
@@ -4366,7 +4377,7 @@
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>
       <c r="P38" s="3"/>
-      <c r="Q38" s="10"/>
+      <c r="Q38" s="3"/>
       <c r="R38" s="3"/>
       <c r="S38" s="3"/>
       <c r="T38" s="3"/>
@@ -4388,7 +4399,7 @@
       <c r="B39" t="s" s="2">
         <v>89</v>
       </c>
-      <c r="C39" s="10"/>
+      <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
@@ -4402,7 +4413,7 @@
       <c r="N39" s="3"/>
       <c r="O39" s="3"/>
       <c r="P39" s="3"/>
-      <c r="Q39" s="10"/>
+      <c r="Q39" s="3"/>
       <c r="R39" s="3"/>
       <c r="S39" s="3"/>
       <c r="T39" s="3"/>
@@ -4424,7 +4435,7 @@
       <c r="B40" t="s" s="2">
         <v>91</v>
       </c>
-      <c r="C40" s="10"/>
+      <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
@@ -4438,7 +4449,7 @@
       <c r="N40" s="3"/>
       <c r="O40" s="3"/>
       <c r="P40" s="3"/>
-      <c r="Q40" s="10"/>
+      <c r="Q40" s="3"/>
       <c r="R40" s="3"/>
       <c r="S40" s="3"/>
       <c r="T40" s="3"/>
@@ -4474,7 +4485,7 @@
       <c r="N41" s="3"/>
       <c r="O41" s="3"/>
       <c r="P41" s="3"/>
-      <c r="Q41" s="10"/>
+      <c r="Q41" s="3"/>
       <c r="R41" s="3"/>
       <c r="S41" s="3"/>
       <c r="T41" s="3"/>
@@ -4496,7 +4507,7 @@
       <c r="B42" t="s" s="2">
         <v>94</v>
       </c>
-      <c r="C42" s="10"/>
+      <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
@@ -4510,7 +4521,7 @@
       <c r="N42" s="3"/>
       <c r="O42" s="3"/>
       <c r="P42" s="3"/>
-      <c r="Q42" s="10"/>
+      <c r="Q42" s="3"/>
       <c r="R42" s="3"/>
       <c r="S42" s="3"/>
       <c r="T42" s="3"/>
@@ -4532,7 +4543,7 @@
       <c r="B43" t="s" s="2">
         <v>19</v>
       </c>
-      <c r="C43" s="10"/>
+      <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
@@ -4546,7 +4557,7 @@
       <c r="N43" s="3"/>
       <c r="O43" s="3"/>
       <c r="P43" s="3"/>
-      <c r="Q43" s="10"/>
+      <c r="Q43" s="3"/>
       <c r="R43" s="3"/>
       <c r="S43" s="3"/>
       <c r="T43" s="3"/>
@@ -4562,13 +4573,13 @@
       <c r="AD43" s="3"/>
     </row>
     <row r="44" ht="17" customHeight="1">
-      <c r="A44" t="s" s="13">
+      <c r="A44" t="s" s="12">
         <v>96</v>
       </c>
-      <c r="B44" t="s" s="14">
+      <c r="B44" t="s" s="13">
         <v>97</v>
       </c>
-      <c r="C44" s="18"/>
+      <c r="C44" s="14"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
@@ -4601,10 +4612,10 @@
       <c r="A45" t="s" s="2">
         <v>98</v>
       </c>
-      <c r="B45" t="s" s="16">
+      <c r="B45" t="s" s="15">
         <v>99</v>
       </c>
-      <c r="C45" s="10"/>
+      <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" t="s" s="2">
         <v>100</v>
@@ -4674,13 +4685,13 @@
       <c r="AD46" s="3"/>
     </row>
     <row r="47" ht="17" customHeight="1">
-      <c r="A47" t="s" s="19">
+      <c r="A47" t="s" s="17">
         <v>104</v>
       </c>
       <c r="B47" t="s" s="8">
         <v>21</v>
       </c>
-      <c r="C47" s="20"/>
+      <c r="C47" s="9"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
@@ -4713,7 +4724,7 @@
       <c r="A48" t="s" s="2">
         <v>105</v>
       </c>
-      <c r="B48" t="s" s="21">
+      <c r="B48" t="s" s="18">
         <v>106</v>
       </c>
       <c r="C48" s="3"/>
@@ -4752,7 +4763,7 @@
       <c r="B49" t="s" s="2">
         <v>108</v>
       </c>
-      <c r="C49" s="10"/>
+      <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
@@ -4862,7 +4873,7 @@
       <c r="B52" t="s" s="2">
         <v>115</v>
       </c>
-      <c r="C52" s="10"/>
+      <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
@@ -4972,7 +4983,7 @@
       <c r="B55" t="s" s="2">
         <v>121</v>
       </c>
-      <c r="C55" s="10"/>
+      <c r="C55" s="3"/>
       <c r="D55" t="s" s="2">
         <v>42</v>
       </c>
@@ -5118,7 +5129,7 @@
       <c r="B59" t="s" s="2">
         <v>126</v>
       </c>
-      <c r="C59" s="10"/>
+      <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
@@ -5264,7 +5275,7 @@
       <c r="B63" t="s" s="2">
         <v>133</v>
       </c>
-      <c r="C63" s="10"/>
+      <c r="C63" s="3"/>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
       <c r="F63" t="s" s="2">
@@ -5302,7 +5313,7 @@
       <c r="B64" t="s" s="2">
         <v>136</v>
       </c>
-      <c r="C64" s="10"/>
+      <c r="C64" s="3"/>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
       <c r="F64" t="s" s="2">
@@ -5370,13 +5381,13 @@
       <c r="AD65" s="3"/>
     </row>
     <row r="66" ht="17" customHeight="1">
-      <c r="A66" t="s" s="13">
+      <c r="A66" t="s" s="12">
         <v>139</v>
       </c>
-      <c r="B66" t="s" s="14">
+      <c r="B66" t="s" s="13">
         <v>140</v>
       </c>
-      <c r="C66" s="18"/>
+      <c r="C66" s="14"/>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
@@ -5409,10 +5420,10 @@
       <c r="A67" t="s" s="2">
         <v>141</v>
       </c>
-      <c r="B67" t="s" s="16">
+      <c r="B67" t="s" s="15">
         <v>142</v>
       </c>
-      <c r="C67" s="10"/>
+      <c r="C67" s="3"/>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
@@ -5520,7 +5531,7 @@
       <c r="B70" t="s" s="2">
         <v>148</v>
       </c>
-      <c r="C70" s="10"/>
+      <c r="C70" s="3"/>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
@@ -5556,7 +5567,7 @@
       <c r="B71" t="s" s="2">
         <v>150</v>
       </c>
-      <c r="C71" s="10"/>
+      <c r="C71" s="3"/>
       <c r="D71" s="3"/>
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
@@ -5592,7 +5603,7 @@
       <c r="B72" t="s" s="2">
         <v>117</v>
       </c>
-      <c r="C72" s="10"/>
+      <c r="C72" s="3"/>
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
@@ -5628,7 +5639,7 @@
       <c r="B73" t="s" s="2">
         <v>153</v>
       </c>
-      <c r="C73" s="10"/>
+      <c r="C73" s="3"/>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
@@ -5664,7 +5675,7 @@
       <c r="B74" t="s" s="2">
         <v>155</v>
       </c>
-      <c r="C74" s="10"/>
+      <c r="C74" s="3"/>
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
@@ -5700,7 +5711,7 @@
       <c r="B75" t="s" s="2">
         <v>136</v>
       </c>
-      <c r="C75" s="10"/>
+      <c r="C75" s="3"/>
       <c r="D75" s="3"/>
       <c r="E75" t="s" s="2">
         <v>157</v>
@@ -5738,7 +5749,7 @@
       <c r="B76" t="s" s="2">
         <v>159</v>
       </c>
-      <c r="C76" s="10"/>
+      <c r="C76" s="3"/>
       <c r="D76" s="3"/>
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
@@ -5776,7 +5787,7 @@
       <c r="B77" t="s" s="2">
         <v>159</v>
       </c>
-      <c r="C77" s="10"/>
+      <c r="C77" s="3"/>
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
       <c r="F77" s="3"/>
@@ -5814,7 +5825,7 @@
       <c r="B78" t="s" s="2">
         <v>121</v>
       </c>
-      <c r="C78" s="10"/>
+      <c r="C78" s="3"/>
       <c r="D78" t="s" s="2">
         <v>51</v>
       </c>
@@ -5852,7 +5863,7 @@
       <c r="B79" t="s" s="2">
         <v>165</v>
       </c>
-      <c r="C79" s="10"/>
+      <c r="C79" s="3"/>
       <c r="D79" s="3"/>
       <c r="E79" s="3"/>
       <c r="F79" s="3"/>
@@ -5888,7 +5899,7 @@
       <c r="B80" t="s" s="2">
         <v>167</v>
       </c>
-      <c r="C80" s="10"/>
+      <c r="C80" s="3"/>
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
@@ -5924,7 +5935,7 @@
       <c r="B81" t="s" s="2">
         <v>67</v>
       </c>
-      <c r="C81" s="22"/>
+      <c r="C81" s="19"/>
       <c r="D81" s="3"/>
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
@@ -5957,13 +5968,13 @@
       <c r="A82" t="s" s="2">
         <v>169</v>
       </c>
-      <c r="B82" t="s" s="19">
+      <c r="B82" t="s" s="17">
         <v>115</v>
       </c>
       <c r="C82" t="s" s="8">
         <v>21</v>
       </c>
-      <c r="D82" s="20"/>
+      <c r="D82" s="9"/>
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
       <c r="G82" s="3"/>
@@ -5998,7 +6009,7 @@
       <c r="B83" t="s" s="2">
         <v>171</v>
       </c>
-      <c r="C83" s="11"/>
+      <c r="C83" s="10"/>
       <c r="D83" s="3"/>
       <c r="E83" s="3"/>
       <c r="F83" t="s" s="2">
@@ -6036,7 +6047,7 @@
       <c r="B84" t="s" s="2">
         <v>174</v>
       </c>
-      <c r="C84" s="10"/>
+      <c r="C84" s="3"/>
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
       <c r="F84" s="3"/>
@@ -6180,7 +6191,7 @@
       <c r="B88" t="s" s="2">
         <v>57</v>
       </c>
-      <c r="C88" s="10"/>
+      <c r="C88" s="3"/>
       <c r="D88" s="3"/>
       <c r="E88" s="3"/>
       <c r="F88" s="3"/>
@@ -6216,7 +6227,7 @@
       <c r="B89" t="s" s="2">
         <v>181</v>
       </c>
-      <c r="C89" s="10"/>
+      <c r="C89" s="3"/>
       <c r="D89" s="3"/>
       <c r="E89" s="3"/>
       <c r="F89" s="3"/>
@@ -6324,7 +6335,7 @@
       <c r="B92" t="s" s="2">
         <v>69</v>
       </c>
-      <c r="C92" s="10"/>
+      <c r="C92" s="3"/>
       <c r="D92" t="s" s="2">
         <v>51</v>
       </c>
@@ -6362,7 +6373,7 @@
       <c r="B93" t="s" s="2">
         <v>187</v>
       </c>
-      <c r="C93" s="10"/>
+      <c r="C93" s="3"/>
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
       <c r="F93" s="3"/>
@@ -6398,7 +6409,7 @@
       <c r="B94" t="s" s="2">
         <v>189</v>
       </c>
-      <c r="C94" s="10"/>
+      <c r="C94" s="3"/>
       <c r="D94" s="3"/>
       <c r="E94" s="3"/>
       <c r="F94" s="3"/>
@@ -6621,7 +6632,7 @@
     </row>
     <row r="101" ht="17" customHeight="1">
       <c r="A101" s="3"/>
-      <c r="B101" s="10"/>
+      <c r="B101" s="3"/>
       <c r="C101" s="3"/>
       <c r="D101" s="3"/>
       <c r="E101" s="3"/>
@@ -6749,7 +6760,7 @@
     </row>
     <row r="105" ht="17" customHeight="1">
       <c r="A105" s="3"/>
-      <c r="B105" s="10"/>
+      <c r="B105" s="3"/>
       <c r="C105" s="3"/>
       <c r="D105" s="3"/>
       <c r="E105" s="3"/>
@@ -6781,7 +6792,7 @@
     </row>
     <row r="106" ht="17" customHeight="1">
       <c r="A106" s="3"/>
-      <c r="B106" s="10"/>
+      <c r="B106" s="3"/>
       <c r="C106" s="3"/>
       <c r="D106" s="3"/>
       <c r="E106" s="3"/>
@@ -6813,7 +6824,7 @@
     </row>
     <row r="107" ht="17" customHeight="1">
       <c r="A107" s="3"/>
-      <c r="B107" s="10"/>
+      <c r="B107" s="3"/>
       <c r="C107" s="3"/>
       <c r="D107" s="3"/>
       <c r="E107" s="3"/>
@@ -6845,7 +6856,7 @@
     </row>
     <row r="108" ht="17" customHeight="1">
       <c r="A108" s="3"/>
-      <c r="B108" s="10"/>
+      <c r="B108" s="3"/>
       <c r="C108" s="3"/>
       <c r="D108" s="3"/>
       <c r="E108" s="3"/>
@@ -6909,7 +6920,7 @@
     </row>
     <row r="110" ht="17" customHeight="1">
       <c r="A110" s="3"/>
-      <c r="B110" s="10"/>
+      <c r="B110" s="3"/>
       <c r="C110" s="3"/>
       <c r="D110" s="3"/>
       <c r="E110" s="3"/>
@@ -6941,7 +6952,7 @@
     </row>
     <row r="111" ht="17" customHeight="1">
       <c r="A111" s="3"/>
-      <c r="B111" s="10"/>
+      <c r="B111" s="3"/>
       <c r="C111" s="3"/>
       <c r="D111" s="3"/>
       <c r="E111" s="3"/>
@@ -6988,19 +6999,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7143" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="10.8672" style="23" customWidth="1"/>
-    <col min="2" max="2" width="10.7344" style="23" customWidth="1"/>
-    <col min="3" max="3" width="10.7344" style="23" customWidth="1"/>
-    <col min="4" max="4" width="10.7344" style="23" customWidth="1"/>
-    <col min="5" max="5" width="10.7344" style="23" customWidth="1"/>
-    <col min="6" max="256" width="10.7344" style="23" customWidth="1"/>
+    <col min="1" max="1" width="10.8672" style="20" customWidth="1"/>
+    <col min="2" max="2" width="10.7344" style="20" customWidth="1"/>
+    <col min="3" max="3" width="10.7344" style="20" customWidth="1"/>
+    <col min="4" max="4" width="10.7344" style="20" customWidth="1"/>
+    <col min="5" max="5" width="10.7344" style="20" customWidth="1"/>
+    <col min="6" max="256" width="10.7344" style="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>190</v>
       </c>
-      <c r="B1" t="s" s="24">
+      <c r="B1" t="s" s="2">
         <v>191</v>
       </c>
       <c r="C1" s="3"/>
@@ -7052,13 +7063,13 @@
       <c r="E5" s="3"/>
     </row>
     <row r="6" ht="17" customHeight="1">
-      <c r="A6" t="s" s="19">
+      <c r="A6" t="s" s="17">
         <v>199</v>
       </c>
-      <c r="B6" t="s" s="25">
+      <c r="B6" t="s" s="21">
         <v>21</v>
       </c>
-      <c r="C6" s="20"/>
+      <c r="C6" s="9"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
@@ -7066,7 +7077,7 @@
       <c r="A7" t="s" s="2">
         <v>200</v>
       </c>
-      <c r="B7" t="s" s="21">
+      <c r="B7" t="s" s="18">
         <v>200</v>
       </c>
       <c r="C7" s="3"/>
@@ -7206,13 +7217,13 @@
       <c r="E19" s="3"/>
     </row>
     <row r="20" ht="17" customHeight="1">
-      <c r="A20" t="s" s="19">
+      <c r="A20" t="s" s="17">
         <v>223</v>
       </c>
-      <c r="B20" t="s" s="25">
+      <c r="B20" t="s" s="21">
         <v>21</v>
       </c>
-      <c r="C20" s="20"/>
+      <c r="C20" s="9"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
@@ -7220,7 +7231,7 @@
       <c r="A21" t="s" s="2">
         <v>224</v>
       </c>
-      <c r="B21" t="s" s="21">
+      <c r="B21" t="s" s="18">
         <v>224</v>
       </c>
       <c r="C21" s="3"/>
@@ -7264,7 +7275,7 @@
       <c r="A25" t="s" s="2">
         <v>230</v>
       </c>
-      <c r="B25" t="s" s="12">
+      <c r="B25" t="s" s="11">
         <v>207</v>
       </c>
       <c r="C25" s="3"/>
@@ -7756,13 +7767,13 @@
       <c r="E69" s="3"/>
     </row>
     <row r="70" ht="17" customHeight="1">
-      <c r="A70" t="s" s="19">
+      <c r="A70" t="s" s="17">
         <v>308</v>
       </c>
-      <c r="B70" t="s" s="25">
+      <c r="B70" t="s" s="21">
         <v>21</v>
       </c>
-      <c r="C70" s="20"/>
+      <c r="C70" s="9"/>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
     </row>
@@ -7770,7 +7781,7 @@
       <c r="A71" t="s" s="2">
         <v>309</v>
       </c>
-      <c r="B71" t="s" s="21">
+      <c r="B71" t="s" s="18">
         <v>309</v>
       </c>
       <c r="C71" s="3"/>
@@ -7792,7 +7803,7 @@
       <c r="A73" t="s" s="2">
         <v>312</v>
       </c>
-      <c r="B73" t="s" s="12">
+      <c r="B73" t="s" s="11">
         <v>313</v>
       </c>
       <c r="C73" s="3"/>
@@ -8001,7 +8012,7 @@
       <c r="A92" t="s" s="2">
         <v>347</v>
       </c>
-      <c r="B92" t="s" s="12">
+      <c r="B92" t="s" s="11">
         <v>313</v>
       </c>
       <c r="C92" s="3"/>
@@ -8144,7 +8155,7 @@
       <c r="A105" t="s" s="2">
         <v>370</v>
       </c>
-      <c r="B105" t="s" s="12">
+      <c r="B105" t="s" s="11">
         <v>313</v>
       </c>
       <c r="C105" s="3"/>
@@ -8276,7 +8287,7 @@
       <c r="A117" t="s" s="2">
         <v>387</v>
       </c>
-      <c r="B117" t="s" s="12">
+      <c r="B117" t="s" s="11">
         <v>207</v>
       </c>
       <c r="C117" s="3"/>
@@ -8311,19 +8322,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7143" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="10.7344" style="26" customWidth="1"/>
-    <col min="2" max="2" width="10.7344" style="26" customWidth="1"/>
-    <col min="3" max="3" width="10.7344" style="26" customWidth="1"/>
-    <col min="4" max="4" width="10.7344" style="26" customWidth="1"/>
-    <col min="5" max="5" width="10.7344" style="26" customWidth="1"/>
-    <col min="6" max="256" width="10.7344" style="26" customWidth="1"/>
+    <col min="1" max="1" width="10.7344" style="22" customWidth="1"/>
+    <col min="2" max="2" width="61.3828" style="22" customWidth="1"/>
+    <col min="3" max="3" width="10.7344" style="22" customWidth="1"/>
+    <col min="4" max="4" width="10.7344" style="22" customWidth="1"/>
+    <col min="5" max="5" width="10.7344" style="22" customWidth="1"/>
+    <col min="6" max="256" width="10.7344" style="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>390</v>
       </c>
-      <c r="B1" t="s" s="24">
+      <c r="B1" t="s" s="2">
         <v>191</v>
       </c>
       <c r="C1" s="3"/>
@@ -8793,6 +8804,11 @@
       <c r="E43" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" location="" tooltip="" display=""/>
+    <hyperlink ref="B8" r:id="rId2" location="" tooltip="" display=""/>
+    <hyperlink ref="B9" r:id="rId3" location="" tooltip="" display=""/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>

</xml_diff>

<commit_message>
CoralTraits mapping - new Kd unit kilo dalton
</commit_message>
<xml_diff>
--- a/Coraltraits/coraltraits_mapping.xlsx
+++ b/Coraltraits/coraltraits_mapping.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="473">
   <si>
     <t>SPECIAL CASES</t>
   </si>
@@ -1451,6 +1451,20 @@
   </si>
   <si>
     <t>years</t>
+  </si>
+  <si>
+    <t>Kd</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="13"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>http://purl.obolibrary.org/obo/UO_0000222</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -8298,7 +8312,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -8783,11 +8797,23 @@
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
     </row>
+    <row r="44" ht="17" customHeight="1">
+      <c r="A44" t="s" s="2">
+        <v>471</v>
+      </c>
+      <c r="B44" t="s" s="2">
+        <v>472</v>
+      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" location="" tooltip="" display="http://eol.org/schema/terms/µmol_cm-2_hr-1"/>
     <hyperlink ref="B8" r:id="rId2" location="" tooltip="" display="http://eol.org/schema/terms/µmol_cm-2_hr-1"/>
     <hyperlink ref="B9" r:id="rId3" location="" tooltip="" display="http://eol.org/schema/terms/µmol_m-2_s-1"/>
+    <hyperlink ref="B44" r:id="rId4" location="" tooltip="" display="http://purl.obolibrary.org/obo/UO_0000222"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>